<commit_message>
write list to ws and save wb
</commit_message>
<xml_diff>
--- a/my_result.xlsx
+++ b/my_result.xlsx
@@ -15,7 +15,43 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>00DataAA</t>
+  </si>
+  <si>
+    <t>01DataAA</t>
+  </si>
+  <si>
+    <t>02DataAA</t>
+  </si>
+  <si>
+    <t>03DataAA</t>
+  </si>
+  <si>
+    <t>04DataAA</t>
+  </si>
+  <si>
+    <t>05DataAA</t>
+  </si>
+  <si>
+    <t>06DataAA</t>
+  </si>
+  <si>
+    <t>07DataAA</t>
+  </si>
+  <si>
+    <t>08DataAA</t>
+  </si>
+  <si>
+    <t>09DataAA</t>
+  </si>
   <si>
     <t>a1-1</t>
   </si>
@@ -28,12 +64,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="맑은 고딕"/>
+      <charset val="129"/>
+      <family val="3"/>
+      <sz val="8"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -61,9 +104,25 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" name="표준" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9">
+    <tableStyle count="1" name="MySqlDefault" pivot="0" table="0">
+      <tableStyleElement dxfId="0" type="headerRow"/>
+    </tableStyle>
+  </tableStyles>
 </styleSheet>
 </file>
 
@@ -356,14 +415,191 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A2:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="n">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="n">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="n">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="n">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="n">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="n">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="n">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="n">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="n">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="n">
+        <v>1</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="n">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="n">
+        <v>3</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="n">
+        <v>4</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="n">
+        <v>5</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="n">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="n">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="n">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="n">
+        <v>9</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
@@ -380,14 +616,14 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C1">
         <f>1+1</f>

</xml_diff>